<commit_message>
Implemented spotify API for audio features, Genius API for lyrics. Refactored file structure
</commit_message>
<xml_diff>
--- a/dataset/output_skladba.xlsx
+++ b/dataset/output_skladba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirko\PycharmProjects\music-and-lyrics-rs\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E553EF-DC56-44F3-969A-55BAD762315A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0209D32C-9697-48B8-A199-559ACE45A02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="231">
   <si>
     <t>ritem</t>
   </si>
@@ -166,15 +166,6 @@
     <t>Barry Manilow: Looks Like We Made It</t>
   </si>
   <si>
-    <t>Beach Boys: God Only Knows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatles: Hey Jude </t>
-  </si>
-  <si>
-    <t>Beatles: Yesterday</t>
-  </si>
-  <si>
     <t>Bee Gees: How Deep Is Your Love</t>
   </si>
   <si>
@@ -191,9 +182,6 @@
   </si>
   <si>
     <t>Blue Swede: Hooked On A Feeling</t>
-  </si>
-  <si>
-    <t>Bo Donaldson And The Heywoods: Billy Don't Be A Hero</t>
   </si>
   <si>
     <t>Bob Dylan: I Shall Be Released</t>
@@ -233,9 +221,6 @@
   </si>
   <si>
     <t>Carpenters: They Long To Be (Close To You)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celine Dion: My Heart Will Go on </t>
   </si>
   <si>
     <t>Christina Aguilera: Beautiful</t>
@@ -343,9 +328,6 @@
     <t>Huey Lewis &amp; The News: The Power Of Love</t>
   </si>
   <si>
-    <t>Human League: Don't You Want Me</t>
-  </si>
-  <si>
     <t>Irene Cara: Flashdance • What a Feeling</t>
   </si>
   <si>
@@ -382,9 +364,6 @@
     <t>Johnny Tillotson: It Keeps Right On A Hurtin</t>
   </si>
   <si>
-    <t>Judy Collis: Send in the Clowns</t>
-  </si>
-  <si>
     <t>Katy Perry: I Kissed A Girl</t>
   </si>
   <si>
@@ -413,9 +392,6 @@
   </si>
   <si>
     <t>Los Del Rio: Macarena</t>
-  </si>
-  <si>
-    <t>MY HUMPS: THE BLACK EYED PEAS</t>
   </si>
   <si>
     <t>Madonna: Like a Prayer</t>
@@ -490,9 +466,6 @@
     <t>Peter Cetera: Glory Of Love</t>
   </si>
   <si>
-    <t>Pink: Who knew</t>
-  </si>
-  <si>
     <t>Pitbull: I know you want me</t>
   </si>
   <si>
@@ -505,22 +478,13 @@
     <t>Queen: Bohemian Rhapsody</t>
   </si>
   <si>
-    <t>R.E.M: Shiny Happy People</t>
-  </si>
-  <si>
     <t xml:space="preserve">Radiohead: Karma Police </t>
   </si>
   <si>
     <t>Rick Springfield: Jessie's Girl</t>
   </si>
   <si>
-    <t>Ricky Martion : Livin La Vida Loca</t>
-  </si>
-  <si>
     <t>Right Said Fred: I'm Too Sexy</t>
-  </si>
-  <si>
-    <t>Rihanna feat. Jay-Z: Umbrella</t>
   </si>
   <si>
     <t xml:space="preserve">Rihanna: Disturbia </t>
@@ -547,19 +511,7 @@
     <t>Sean Kingston: Fire Burning</t>
   </si>
   <si>
-    <t>Sergio Mendes: Never Gonna Let You Go</t>
-  </si>
-  <si>
     <t>Shakira: Whenever, Wherever</t>
-  </si>
-  <si>
-    <t>Sinead O'Connor: Nothing Compares 2 U</t>
-  </si>
-  <si>
-    <t>Sonny and Cher: The beat goes on</t>
-  </si>
-  <si>
-    <t>Speedy Gonzales: Pat Boone</t>
   </si>
   <si>
     <t>Spice Girls: Wannabe</t>
@@ -590,9 +542,6 @@
   </si>
   <si>
     <t>The Beatles: All You Need Is Love</t>
-  </si>
-  <si>
-    <t>The Black Eyed Peas: I Gotta Feeling</t>
   </si>
   <si>
     <t>The Doors: Hello, I Love You</t>
@@ -655,9 +604,6 @@
     <t>Train: Drops of Jupiter</t>
   </si>
   <si>
-    <t>USA For Africa: We Are The World</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ultravox : Vienna </t>
   </si>
   <si>
@@ -691,9 +637,6 @@
     <t>Bob Dylan: A Hard Rain's A-Gonna Fall</t>
   </si>
   <si>
-    <t>NSYNC: It's Gonna Be Me</t>
-  </si>
-  <si>
     <t>UB40: (I Can’t Help) Falling in Love With You</t>
   </si>
   <si>
@@ -716,6 +659,60 @@
   </si>
   <si>
     <t>John Lennon: Love</t>
+  </si>
+  <si>
+    <t>The Beach Boys: God Only Knows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Beatles: Hey Jude </t>
+  </si>
+  <si>
+    <t>The Beatles: Yesterday</t>
+  </si>
+  <si>
+    <t>Bo Donaldson &amp; The Heywoods: Billy, Don't Be A Hero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Céline Dion: My Heart Will Go on </t>
+  </si>
+  <si>
+    <t>Judy Collins: Send in the Clowns</t>
+  </si>
+  <si>
+    <t>P!nk: Who knew</t>
+  </si>
+  <si>
+    <t>R.E.M.: Shiny Happy People</t>
+  </si>
+  <si>
+    <t>Ricky Martin : Livin La Vida Loca</t>
+  </si>
+  <si>
+    <t>Rihanna: Umbrella</t>
+  </si>
+  <si>
+    <t>Sérgio Mendes: Never Gonna Let You Go</t>
+  </si>
+  <si>
+    <t>Sinéad O'Connor: Nothing Compares 2 U</t>
+  </si>
+  <si>
+    <t>Sonny &amp; Cher: The beat goes on</t>
+  </si>
+  <si>
+    <t>Pat Boone: Speedy Gonzales</t>
+  </si>
+  <si>
+    <t>BLACK EYED PEAS: MY HUMPS</t>
+  </si>
+  <si>
+    <t>Black Eyed Peas: I Gotta Feeling</t>
+  </si>
+  <si>
+    <t>U.S.A. For Africa: We Are The World</t>
+  </si>
+  <si>
+    <t>*NSYNC: It's Gonna Be Me</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4708,7 +4705,7 @@
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -5772,7 +5769,7 @@
     </row>
     <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>213</v>
       </c>
       <c r="B20">
         <v>3.25</v>
@@ -6038,7 +6035,7 @@
     </row>
     <row r="21" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>214</v>
       </c>
       <c r="B21">
         <v>2.25</v>
@@ -6304,7 +6301,7 @@
     </row>
     <row r="22" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
       <c r="B22">
         <v>2.666666666666667</v>
@@ -6570,7 +6567,7 @@
     </row>
     <row r="23" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -6836,7 +6833,7 @@
     </row>
     <row r="24" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -7102,7 +7099,7 @@
     </row>
     <row r="25" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>1.8</v>
@@ -7368,7 +7365,7 @@
     </row>
     <row r="26" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -7634,7 +7631,7 @@
     </row>
     <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -7900,7 +7897,7 @@
     </row>
     <row r="28" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>1.8</v>
@@ -8166,7 +8163,7 @@
     </row>
     <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>216</v>
       </c>
       <c r="B29">
         <v>3.2</v>
@@ -8432,7 +8429,7 @@
     </row>
     <row r="30" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>2.25</v>
@@ -8698,7 +8695,7 @@
     </row>
     <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="B31">
         <v>2.5</v>
@@ -8964,7 +8961,7 @@
     </row>
     <row r="32" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>1.75</v>
@@ -9230,7 +9227,7 @@
     </row>
     <row r="33" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>3.25</v>
@@ -9496,7 +9493,7 @@
     </row>
     <row r="34" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>1.333333333333333</v>
@@ -9762,7 +9759,7 @@
     </row>
     <row r="35" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>2.5</v>
@@ -10028,7 +10025,7 @@
     </row>
     <row r="36" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>3.75</v>
@@ -10294,7 +10291,7 @@
     </row>
     <row r="37" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37">
         <v>2.5</v>
@@ -10560,7 +10557,7 @@
     </row>
     <row r="38" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <v>1.75</v>
@@ -10826,7 +10823,7 @@
     </row>
     <row r="39" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -11092,7 +11089,7 @@
     </row>
     <row r="40" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B40">
         <v>3.25</v>
@@ -11358,7 +11355,7 @@
     </row>
     <row r="41" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B41">
         <v>2.333333333333333</v>
@@ -11624,7 +11621,7 @@
     </row>
     <row r="42" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="B42">
         <v>1.75</v>
@@ -11890,7 +11887,7 @@
     </row>
     <row r="43" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B43">
         <v>2.75</v>
@@ -12156,7 +12153,7 @@
     </row>
     <row r="44" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B44">
         <v>2.4</v>
@@ -12422,7 +12419,7 @@
     </row>
     <row r="45" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -12688,7 +12685,7 @@
     </row>
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>217</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -12954,7 +12951,7 @@
     </row>
     <row r="47" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B47">
         <v>1.6</v>
@@ -13220,7 +13217,7 @@
     </row>
     <row r="48" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -13486,7 +13483,7 @@
     </row>
     <row r="49" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>2.25</v>
@@ -13752,7 +13749,7 @@
     </row>
     <row r="50" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -14018,7 +14015,7 @@
     </row>
     <row r="51" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B51">
         <v>2.75</v>
@@ -14284,7 +14281,7 @@
     </row>
     <row r="52" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -14550,7 +14547,7 @@
     </row>
     <row r="53" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -14816,7 +14813,7 @@
     </row>
     <row r="54" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B54">
         <v>2.25</v>
@@ -15082,7 +15079,7 @@
     </row>
     <row r="55" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B55">
         <v>2.6</v>
@@ -15348,7 +15345,7 @@
     </row>
     <row r="56" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B56">
         <v>2.666666666666667</v>
@@ -15614,7 +15611,7 @@
     </row>
     <row r="57" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -15880,7 +15877,7 @@
     </row>
     <row r="58" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -16146,7 +16143,7 @@
     </row>
     <row r="59" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -16412,7 +16409,7 @@
     </row>
     <row r="60" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -16678,7 +16675,7 @@
     </row>
     <row r="61" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B61">
         <v>2.75</v>
@@ -16944,7 +16941,7 @@
     </row>
     <row r="62" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B62">
         <v>2.5</v>
@@ -17210,7 +17207,7 @@
     </row>
     <row r="63" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -17476,7 +17473,7 @@
     </row>
     <row r="64" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B64">
         <v>2.5</v>
@@ -17742,7 +17739,7 @@
     </row>
     <row r="65" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B65">
         <v>2.666666666666667</v>
@@ -18008,7 +18005,7 @@
     </row>
     <row r="66" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -18274,7 +18271,7 @@
     </row>
     <row r="67" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B67">
         <v>2.2000000000000002</v>
@@ -18540,7 +18537,7 @@
     </row>
     <row r="68" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B68">
         <v>2.5</v>
@@ -18806,7 +18803,7 @@
     </row>
     <row r="69" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B69">
         <v>2.25</v>
@@ -19072,7 +19069,7 @@
     </row>
     <row r="70" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="B70">
         <v>2.5</v>
@@ -19338,7 +19335,7 @@
     </row>
     <row r="71" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B71">
         <v>1.75</v>
@@ -19604,7 +19601,7 @@
     </row>
     <row r="72" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B72">
         <v>1.5</v>
@@ -19870,7 +19867,7 @@
     </row>
     <row r="73" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B73">
         <v>2.5</v>
@@ -20136,7 +20133,7 @@
     </row>
     <row r="74" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -20402,7 +20399,7 @@
     </row>
     <row r="75" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B75">
         <v>2.6</v>
@@ -20668,7 +20665,7 @@
     </row>
     <row r="76" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -20934,7 +20931,7 @@
     </row>
     <row r="77" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B77">
         <v>1.75</v>
@@ -21200,7 +21197,7 @@
     </row>
     <row r="78" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B78">
         <v>1.8</v>
@@ -21466,7 +21463,7 @@
     </row>
     <row r="79" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B79">
         <v>2.5</v>
@@ -21732,7 +21729,7 @@
     </row>
     <row r="80" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B80">
         <v>2.25</v>
@@ -21998,7 +21995,7 @@
     </row>
     <row r="81" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -22264,7 +22261,7 @@
     </row>
     <row r="82" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -22530,7 +22527,7 @@
     </row>
     <row r="83" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -22709,7 +22706,7 @@
     </row>
     <row r="84" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B84">
         <v>3</v>
@@ -22975,7 +22972,7 @@
     </row>
     <row r="85" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B85">
         <v>3</v>
@@ -23241,7 +23238,7 @@
     </row>
     <row r="86" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B86">
         <v>1.75</v>
@@ -23507,7 +23504,7 @@
     </row>
     <row r="87" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B87">
         <v>4</v>
@@ -23773,7 +23770,7 @@
     </row>
     <row r="88" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="B88">
         <v>4</v>
@@ -24039,7 +24036,7 @@
     </row>
     <row r="89" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B89">
         <v>2.333333333333333</v>
@@ -24305,7 +24302,7 @@
     </row>
     <row r="90" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B90">
         <v>2.8</v>
@@ -24571,7 +24568,7 @@
     </row>
     <row r="91" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -24837,7 +24834,7 @@
     </row>
     <row r="92" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B92">
         <v>2.25</v>
@@ -25103,7 +25100,7 @@
     </row>
     <row r="93" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -25282,7 +25279,7 @@
     </row>
     <row r="94" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B94">
         <v>2.25</v>
@@ -25548,7 +25545,7 @@
     </row>
     <row r="95" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B95">
         <v>2.25</v>
@@ -25814,7 +25811,7 @@
     </row>
     <row r="96" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B96">
         <v>2</v>
@@ -26080,7 +26077,7 @@
     </row>
     <row r="97" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -26346,7 +26343,7 @@
     </row>
     <row r="98" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B98">
         <v>2.25</v>
@@ -26612,7 +26609,7 @@
     </row>
     <row r="99" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B99">
         <v>1.75</v>
@@ -26878,7 +26875,7 @@
     </row>
     <row r="100" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B100">
         <v>1.5</v>
@@ -27144,7 +27141,7 @@
     </row>
     <row r="101" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B101">
         <v>1.75</v>
@@ -27410,7 +27407,7 @@
     </row>
     <row r="102" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>120</v>
+        <v>218</v>
       </c>
       <c r="B102">
         <v>3.25</v>
@@ -27676,7 +27673,7 @@
     </row>
     <row r="103" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B103">
         <v>1.8</v>
@@ -27942,7 +27939,7 @@
     </row>
     <row r="104" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B104">
         <v>3.5</v>
@@ -28208,7 +28205,7 @@
     </row>
     <row r="105" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B105">
         <v>2</v>
@@ -28474,7 +28471,7 @@
     </row>
     <row r="106" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B106">
         <v>2</v>
@@ -28740,7 +28737,7 @@
     </row>
     <row r="107" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B107">
         <v>1.333333333333333</v>
@@ -29006,7 +29003,7 @@
     </row>
     <row r="108" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -29272,7 +29269,7 @@
     </row>
     <row r="109" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B109">
         <v>2.666666666666667</v>
@@ -29538,7 +29535,7 @@
     </row>
     <row r="110" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -29804,7 +29801,7 @@
     </row>
     <row r="111" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B111">
         <v>2.5</v>
@@ -30070,7 +30067,7 @@
     </row>
     <row r="112" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B112">
         <v>1.75</v>
@@ -30336,7 +30333,7 @@
     </row>
     <row r="113" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>131</v>
+        <v>227</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -30602,7 +30599,7 @@
     </row>
     <row r="114" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B114">
         <v>2.75</v>
@@ -30868,7 +30865,7 @@
     </row>
     <row r="115" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B115">
         <v>2.333333333333333</v>
@@ -31134,7 +31131,7 @@
     </row>
     <row r="116" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B116">
         <v>1.333333333333333</v>
@@ -31400,7 +31397,7 @@
     </row>
     <row r="117" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -31666,7 +31663,7 @@
     </row>
     <row r="118" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -31932,7 +31929,7 @@
     </row>
     <row r="119" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B119">
         <v>2.5</v>
@@ -32198,7 +32195,7 @@
     </row>
     <row r="120" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B120">
         <v>3.333333333333333</v>
@@ -32464,7 +32461,7 @@
     </row>
     <row r="121" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -32730,7 +32727,7 @@
     </row>
     <row r="122" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -32996,7 +32993,7 @@
     </row>
     <row r="123" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B123">
         <v>1.75</v>
@@ -33262,7 +33259,7 @@
     </row>
     <row r="124" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B124">
         <v>3.4</v>
@@ -33528,7 +33525,7 @@
     </row>
     <row r="125" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B125">
         <v>1.5</v>
@@ -33794,7 +33791,7 @@
     </row>
     <row r="126" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -33973,7 +33970,7 @@
     </row>
     <row r="127" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B127">
         <v>3.5</v>
@@ -34239,7 +34236,7 @@
     </row>
     <row r="128" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B128">
         <v>2.25</v>
@@ -34505,7 +34502,7 @@
     </row>
     <row r="129" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B129">
         <v>3.25</v>
@@ -34771,7 +34768,7 @@
     </row>
     <row r="130" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B130">
         <v>3.25</v>
@@ -35037,7 +35034,7 @@
     </row>
     <row r="131" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B131">
         <v>3.25</v>
@@ -35303,7 +35300,7 @@
     </row>
     <row r="132" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -35569,7 +35566,7 @@
     </row>
     <row r="133" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B133">
         <v>2</v>
@@ -35835,7 +35832,7 @@
     </row>
     <row r="134" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B134">
         <v>1.6</v>
@@ -36101,7 +36098,7 @@
     </row>
     <row r="135" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -36367,7 +36364,7 @@
     </row>
     <row r="136" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B136">
         <v>1.5</v>
@@ -36633,7 +36630,7 @@
     </row>
     <row r="137" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B137">
         <v>3.25</v>
@@ -36899,7 +36896,7 @@
     </row>
     <row r="138" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="B138">
         <v>2.25</v>
@@ -37165,7 +37162,7 @@
     </row>
     <row r="139" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B139">
         <v>3</v>
@@ -37431,7 +37428,7 @@
     </row>
     <row r="140" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B140">
         <v>2.333333333333333</v>
@@ -37697,7 +37694,7 @@
     </row>
     <row r="141" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B141">
         <v>2.5</v>
@@ -37963,7 +37960,7 @@
     </row>
     <row r="142" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B142">
         <v>2.25</v>
@@ -38229,7 +38226,7 @@
     </row>
     <row r="143" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>161</v>
+        <v>220</v>
       </c>
       <c r="B143">
         <v>3</v>
@@ -38495,7 +38492,7 @@
     </row>
     <row r="144" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B144">
         <v>3.333333333333333</v>
@@ -38761,7 +38758,7 @@
     </row>
     <row r="145" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B145">
         <v>2.75</v>
@@ -39027,7 +39024,7 @@
     </row>
     <row r="146" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="B146">
         <v>2</v>
@@ -39293,7 +39290,7 @@
     </row>
     <row r="147" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B147">
         <v>2.75</v>
@@ -39559,7 +39556,7 @@
     </row>
     <row r="148" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="B148">
         <v>2</v>
@@ -39825,7 +39822,7 @@
     </row>
     <row r="149" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B149">
         <v>1.8</v>
@@ -40091,7 +40088,7 @@
     </row>
     <row r="150" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B150">
         <v>2.25</v>
@@ -40357,7 +40354,7 @@
     </row>
     <row r="151" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B151">
         <v>3.75</v>
@@ -40623,7 +40620,7 @@
     </row>
     <row r="152" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B152">
         <v>2.2000000000000002</v>
@@ -40889,7 +40886,7 @@
     </row>
     <row r="153" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B153">
         <v>2</v>
@@ -41155,7 +41152,7 @@
     </row>
     <row r="154" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B154">
         <v>2.6</v>
@@ -41421,7 +41418,7 @@
     </row>
     <row r="155" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B155">
         <v>3.25</v>
@@ -41687,7 +41684,7 @@
     </row>
     <row r="156" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B156">
         <v>2.8</v>
@@ -41953,7 +41950,7 @@
     </row>
     <row r="157" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="B157">
         <v>2</v>
@@ -42219,7 +42216,7 @@
     </row>
     <row r="158" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B158">
         <v>2.25</v>
@@ -42485,7 +42482,7 @@
     </row>
     <row r="159" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="B159">
         <v>1.5</v>
@@ -42751,7 +42748,7 @@
     </row>
     <row r="160" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="B160">
         <v>2</v>
@@ -43017,7 +43014,7 @@
     </row>
     <row r="161" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="B161">
         <v>1.5</v>
@@ -43283,7 +43280,7 @@
     </row>
     <row r="162" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B162">
         <v>1.75</v>
@@ -43549,7 +43546,7 @@
     </row>
     <row r="163" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B163">
         <v>3</v>
@@ -43815,7 +43812,7 @@
     </row>
     <row r="164" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B164">
         <v>2.2000000000000002</v>
@@ -44081,7 +44078,7 @@
     </row>
     <row r="165" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B165">
         <v>2.666666666666667</v>
@@ -44347,7 +44344,7 @@
     </row>
     <row r="166" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B166">
         <v>1.75</v>
@@ -44613,7 +44610,7 @@
     </row>
     <row r="167" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B167">
         <v>3.75</v>
@@ -44879,7 +44876,7 @@
     </row>
     <row r="168" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B168">
         <v>1.25</v>
@@ -45145,7 +45142,7 @@
     </row>
     <row r="169" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B169">
         <v>3</v>
@@ -45411,7 +45408,7 @@
     </row>
     <row r="170" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B170">
         <v>3</v>
@@ -45677,7 +45674,7 @@
     </row>
     <row r="171" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B171">
         <v>1.75</v>
@@ -45943,7 +45940,7 @@
     </row>
     <row r="172" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="B172">
         <v>3.25</v>
@@ -46209,7 +46206,7 @@
     </row>
     <row r="173" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B173">
         <v>2.5</v>
@@ -46475,7 +46472,7 @@
     </row>
     <row r="174" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B174">
         <v>3.25</v>
@@ -46741,7 +46738,7 @@
     </row>
     <row r="175" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="B175">
         <v>3.4</v>
@@ -47007,7 +47004,7 @@
     </row>
     <row r="176" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B176">
         <v>2.25</v>
@@ -47273,7 +47270,7 @@
     </row>
     <row r="177" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B177">
         <v>4</v>
@@ -47539,7 +47536,7 @@
     </row>
     <row r="178" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B178">
         <v>2.5</v>
@@ -47805,7 +47802,7 @@
     </row>
     <row r="179" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="B179">
         <v>2.25</v>
@@ -48071,7 +48068,7 @@
     </row>
     <row r="180" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="B180">
         <v>2.25</v>
@@ -48337,7 +48334,7 @@
     </row>
     <row r="181" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B181">
         <v>3.666666666666667</v>
@@ -48603,7 +48600,7 @@
     </row>
     <row r="182" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B182">
         <v>2.25</v>
@@ -48869,7 +48866,7 @@
     </row>
     <row r="183" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B183">
         <v>4.333333333333333</v>
@@ -49135,7 +49132,7 @@
     </row>
     <row r="184" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="B184">
         <v>2</v>
@@ -49401,7 +49398,7 @@
     </row>
     <row r="185" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B185">
         <v>2.75</v>
@@ -49667,7 +49664,7 @@
     </row>
     <row r="186" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B186">
         <v>2.5</v>
@@ -49933,7 +49930,7 @@
     </row>
     <row r="187" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B187">
         <v>2.5</v>
@@ -50199,7 +50196,7 @@
     </row>
     <row r="188" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B188">
         <v>1.666666666666667</v>
@@ -50465,7 +50462,7 @@
     </row>
     <row r="189" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B189">
         <v>2.5</v>
@@ -50731,7 +50728,7 @@
     </row>
     <row r="190" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B190">
         <v>3.25</v>
@@ -50997,7 +50994,7 @@
     </row>
     <row r="191" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B191">
         <v>2</v>
@@ -51263,7 +51260,7 @@
     </row>
     <row r="192" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B192">
         <v>4.25</v>
@@ -51529,7 +51526,7 @@
     </row>
     <row r="193" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B193">
         <v>2.8</v>
@@ -51795,7 +51792,7 @@
     </row>
     <row r="194" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B194">
         <v>2.4</v>
@@ -52061,7 +52058,7 @@
     </row>
     <row r="195" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="B195">
         <v>4</v>
@@ -52327,7 +52324,7 @@
     </row>
     <row r="196" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B196">
         <v>3.333333333333333</v>
@@ -52593,7 +52590,7 @@
     </row>
     <row r="197" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B197">
         <v>2.6</v>
@@ -52859,7 +52856,7 @@
     </row>
     <row r="198" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="B198">
         <v>2.8</v>
@@ -53125,7 +53122,7 @@
     </row>
     <row r="199" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>2</v>
@@ -53391,7 +53388,7 @@
     </row>
     <row r="200" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>2.25</v>
@@ -53657,7 +53654,7 @@
     </row>
     <row r="201" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B201">
         <v>3</v>
@@ -53923,7 +53920,7 @@
     </row>
     <row r="202" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B202">
         <v>2.25</v>
@@ -54189,6 +54186,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BG1:BI1"/>
     <mergeCell ref="BY1:CA1"/>
     <mergeCell ref="CB1:CD1"/>
     <mergeCell ref="CE1:CG1"/>
@@ -54198,26 +54215,6 @@
     <mergeCell ref="BP1:BR1"/>
     <mergeCell ref="BS1:BU1"/>
     <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="AU1:AW1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="BD1:BF1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Song features evaluating added
</commit_message>
<xml_diff>
--- a/dataset/output_skladba.xlsx
+++ b/dataset/output_skladba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirko\PycharmProjects\music-and-lyrics-rs\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0209D32C-9697-48B8-A199-559ACE45A02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90D6DC5-F6B1-449F-B9A5-4AFB3E599D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Bobby Vinton: Roses Are Red (My Love)</t>
-  </si>
-  <si>
-    <t>Both Sides: Both Sides Now</t>
   </si>
   <si>
     <t>Brian Hyland: Itsy Bitsy Teenie Weenie Yellow Polka Dot Bikini</t>
@@ -714,6 +711,9 @@
   <si>
     <t>*NSYNC: It's Gonna Be Me</t>
   </si>
+  <si>
+    <t>Joni Mitchell: Both Sides Now</t>
+  </si>
 </sst>
 </file>
 
@@ -1085,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CJ202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20">
         <v>3.25</v>
@@ -6035,7 +6035,7 @@
     </row>
     <row r="21" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21">
         <v>2.25</v>
@@ -6301,7 +6301,7 @@
     </row>
     <row r="22" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B22">
         <v>2.666666666666667</v>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B29">
         <v>3.2</v>
@@ -8695,7 +8695,7 @@
     </row>
     <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B31">
         <v>2.5</v>
@@ -10025,7 +10025,7 @@
     </row>
     <row r="36" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>230</v>
       </c>
       <c r="B36">
         <v>3.75</v>
@@ -10291,7 +10291,7 @@
     </row>
     <row r="37" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>2.5</v>
@@ -10557,7 +10557,7 @@
     </row>
     <row r="38" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38">
         <v>1.75</v>
@@ -10823,7 +10823,7 @@
     </row>
     <row r="39" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="40" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40">
         <v>3.25</v>
@@ -11355,7 +11355,7 @@
     </row>
     <row r="41" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>2.333333333333333</v>
@@ -11621,7 +11621,7 @@
     </row>
     <row r="42" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B42">
         <v>1.75</v>
@@ -11887,7 +11887,7 @@
     </row>
     <row r="43" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>2.75</v>
@@ -12153,7 +12153,7 @@
     </row>
     <row r="44" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44">
         <v>2.4</v>
@@ -12419,7 +12419,7 @@
     </row>
     <row r="45" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -12685,7 +12685,7 @@
     </row>
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -12951,7 +12951,7 @@
     </row>
     <row r="47" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47">
         <v>1.6</v>
@@ -13217,7 +13217,7 @@
     </row>
     <row r="48" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -13483,7 +13483,7 @@
     </row>
     <row r="49" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49">
         <v>2.25</v>
@@ -13749,7 +13749,7 @@
     </row>
     <row r="50" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -14015,7 +14015,7 @@
     </row>
     <row r="51" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51">
         <v>2.75</v>
@@ -14281,7 +14281,7 @@
     </row>
     <row r="52" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -14547,7 +14547,7 @@
     </row>
     <row r="53" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -14813,7 +14813,7 @@
     </row>
     <row r="54" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54">
         <v>2.25</v>
@@ -15079,7 +15079,7 @@
     </row>
     <row r="55" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B55">
         <v>2.6</v>
@@ -15345,7 +15345,7 @@
     </row>
     <row r="56" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56">
         <v>2.666666666666667</v>
@@ -15611,7 +15611,7 @@
     </row>
     <row r="57" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -15877,7 +15877,7 @@
     </row>
     <row r="58" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -16143,7 +16143,7 @@
     </row>
     <row r="59" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -16409,7 +16409,7 @@
     </row>
     <row r="60" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -16675,7 +16675,7 @@
     </row>
     <row r="61" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61">
         <v>2.75</v>
@@ -16941,7 +16941,7 @@
     </row>
     <row r="62" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62">
         <v>2.5</v>
@@ -17207,7 +17207,7 @@
     </row>
     <row r="63" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -17473,7 +17473,7 @@
     </row>
     <row r="64" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64">
         <v>2.5</v>
@@ -17739,7 +17739,7 @@
     </row>
     <row r="65" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65">
         <v>2.666666666666667</v>
@@ -18005,7 +18005,7 @@
     </row>
     <row r="66" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -18271,7 +18271,7 @@
     </row>
     <row r="67" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B67">
         <v>2.2000000000000002</v>
@@ -18537,7 +18537,7 @@
     </row>
     <row r="68" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68">
         <v>2.5</v>
@@ -18803,7 +18803,7 @@
     </row>
     <row r="69" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69">
         <v>2.25</v>
@@ -19069,7 +19069,7 @@
     </row>
     <row r="70" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B70">
         <v>2.5</v>
@@ -19335,7 +19335,7 @@
     </row>
     <row r="71" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B71">
         <v>1.75</v>
@@ -19601,7 +19601,7 @@
     </row>
     <row r="72" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B72">
         <v>1.5</v>
@@ -19867,7 +19867,7 @@
     </row>
     <row r="73" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B73">
         <v>2.5</v>
@@ -20133,7 +20133,7 @@
     </row>
     <row r="74" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -20399,7 +20399,7 @@
     </row>
     <row r="75" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B75">
         <v>2.6</v>
@@ -20665,7 +20665,7 @@
     </row>
     <row r="76" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -20931,7 +20931,7 @@
     </row>
     <row r="77" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77">
         <v>1.75</v>
@@ -21197,7 +21197,7 @@
     </row>
     <row r="78" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B78">
         <v>1.8</v>
@@ -21463,7 +21463,7 @@
     </row>
     <row r="79" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B79">
         <v>2.5</v>
@@ -21729,7 +21729,7 @@
     </row>
     <row r="80" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B80">
         <v>2.25</v>
@@ -21995,7 +21995,7 @@
     </row>
     <row r="81" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -22261,7 +22261,7 @@
     </row>
     <row r="82" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -22527,7 +22527,7 @@
     </row>
     <row r="83" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -22706,7 +22706,7 @@
     </row>
     <row r="84" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B84">
         <v>3</v>
@@ -22972,7 +22972,7 @@
     </row>
     <row r="85" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B85">
         <v>3</v>
@@ -23238,7 +23238,7 @@
     </row>
     <row r="86" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B86">
         <v>1.75</v>
@@ -23504,7 +23504,7 @@
     </row>
     <row r="87" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B87">
         <v>4</v>
@@ -23770,7 +23770,7 @@
     </row>
     <row r="88" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88">
         <v>4</v>
@@ -24036,7 +24036,7 @@
     </row>
     <row r="89" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B89">
         <v>2.333333333333333</v>
@@ -24302,7 +24302,7 @@
     </row>
     <row r="90" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90">
         <v>2.8</v>
@@ -24568,7 +24568,7 @@
     </row>
     <row r="91" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -24834,7 +24834,7 @@
     </row>
     <row r="92" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B92">
         <v>2.25</v>
@@ -25100,7 +25100,7 @@
     </row>
     <row r="93" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -25279,7 +25279,7 @@
     </row>
     <row r="94" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94">
         <v>2.25</v>
@@ -25545,7 +25545,7 @@
     </row>
     <row r="95" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95">
         <v>2.25</v>
@@ -25811,7 +25811,7 @@
     </row>
     <row r="96" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B96">
         <v>2</v>
@@ -26077,7 +26077,7 @@
     </row>
     <row r="97" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -26343,7 +26343,7 @@
     </row>
     <row r="98" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B98">
         <v>2.25</v>
@@ -26609,7 +26609,7 @@
     </row>
     <row r="99" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B99">
         <v>1.75</v>
@@ -26875,7 +26875,7 @@
     </row>
     <row r="100" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B100">
         <v>1.5</v>
@@ -27141,7 +27141,7 @@
     </row>
     <row r="101" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B101">
         <v>1.75</v>
@@ -27407,7 +27407,7 @@
     </row>
     <row r="102" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B102">
         <v>3.25</v>
@@ -27673,7 +27673,7 @@
     </row>
     <row r="103" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B103">
         <v>1.8</v>
@@ -27939,7 +27939,7 @@
     </row>
     <row r="104" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B104">
         <v>3.5</v>
@@ -28205,7 +28205,7 @@
     </row>
     <row r="105" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B105">
         <v>2</v>
@@ -28471,7 +28471,7 @@
     </row>
     <row r="106" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B106">
         <v>2</v>
@@ -28737,7 +28737,7 @@
     </row>
     <row r="107" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B107">
         <v>1.333333333333333</v>
@@ -29003,7 +29003,7 @@
     </row>
     <row r="108" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -29269,7 +29269,7 @@
     </row>
     <row r="109" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B109">
         <v>2.666666666666667</v>
@@ -29535,7 +29535,7 @@
     </row>
     <row r="110" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -29801,7 +29801,7 @@
     </row>
     <row r="111" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B111">
         <v>2.5</v>
@@ -30067,7 +30067,7 @@
     </row>
     <row r="112" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B112">
         <v>1.75</v>
@@ -30333,7 +30333,7 @@
     </row>
     <row r="113" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -30599,7 +30599,7 @@
     </row>
     <row r="114" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B114">
         <v>2.75</v>
@@ -30865,7 +30865,7 @@
     </row>
     <row r="115" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B115">
         <v>2.333333333333333</v>
@@ -31131,7 +31131,7 @@
     </row>
     <row r="116" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116">
         <v>1.333333333333333</v>
@@ -31397,7 +31397,7 @@
     </row>
     <row r="117" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -31663,7 +31663,7 @@
     </row>
     <row r="118" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -31929,7 +31929,7 @@
     </row>
     <row r="119" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B119">
         <v>2.5</v>
@@ -32195,7 +32195,7 @@
     </row>
     <row r="120" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120">
         <v>3.333333333333333</v>
@@ -32461,7 +32461,7 @@
     </row>
     <row r="121" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -32727,7 +32727,7 @@
     </row>
     <row r="122" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -32993,7 +32993,7 @@
     </row>
     <row r="123" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123">
         <v>1.75</v>
@@ -33259,7 +33259,7 @@
     </row>
     <row r="124" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B124">
         <v>3.4</v>
@@ -33525,7 +33525,7 @@
     </row>
     <row r="125" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B125">
         <v>1.5</v>
@@ -33791,7 +33791,7 @@
     </row>
     <row r="126" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -33970,7 +33970,7 @@
     </row>
     <row r="127" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127">
         <v>3.5</v>
@@ -34236,7 +34236,7 @@
     </row>
     <row r="128" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B128">
         <v>2.25</v>
@@ -34502,7 +34502,7 @@
     </row>
     <row r="129" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B129">
         <v>3.25</v>
@@ -34768,7 +34768,7 @@
     </row>
     <row r="130" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B130">
         <v>3.25</v>
@@ -35034,7 +35034,7 @@
     </row>
     <row r="131" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B131">
         <v>3.25</v>
@@ -35300,7 +35300,7 @@
     </row>
     <row r="132" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -35566,7 +35566,7 @@
     </row>
     <row r="133" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B133">
         <v>2</v>
@@ -35832,7 +35832,7 @@
     </row>
     <row r="134" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B134">
         <v>1.6</v>
@@ -36098,7 +36098,7 @@
     </row>
     <row r="135" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -36364,7 +36364,7 @@
     </row>
     <row r="136" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B136">
         <v>1.5</v>
@@ -36630,7 +36630,7 @@
     </row>
     <row r="137" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B137">
         <v>3.25</v>
@@ -36896,7 +36896,7 @@
     </row>
     <row r="138" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B138">
         <v>2.25</v>
@@ -37162,7 +37162,7 @@
     </row>
     <row r="139" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B139">
         <v>3</v>
@@ -37428,7 +37428,7 @@
     </row>
     <row r="140" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B140">
         <v>2.333333333333333</v>
@@ -37694,7 +37694,7 @@
     </row>
     <row r="141" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B141">
         <v>2.5</v>
@@ -37960,7 +37960,7 @@
     </row>
     <row r="142" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B142">
         <v>2.25</v>
@@ -38226,7 +38226,7 @@
     </row>
     <row r="143" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B143">
         <v>3</v>
@@ -38492,7 +38492,7 @@
     </row>
     <row r="144" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B144">
         <v>3.333333333333333</v>
@@ -38758,7 +38758,7 @@
     </row>
     <row r="145" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B145">
         <v>2.75</v>
@@ -39024,7 +39024,7 @@
     </row>
     <row r="146" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B146">
         <v>2</v>
@@ -39290,7 +39290,7 @@
     </row>
     <row r="147" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B147">
         <v>2.75</v>
@@ -39556,7 +39556,7 @@
     </row>
     <row r="148" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B148">
         <v>2</v>
@@ -39822,7 +39822,7 @@
     </row>
     <row r="149" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B149">
         <v>1.8</v>
@@ -40088,7 +40088,7 @@
     </row>
     <row r="150" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B150">
         <v>2.25</v>
@@ -40354,7 +40354,7 @@
     </row>
     <row r="151" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B151">
         <v>3.75</v>
@@ -40620,7 +40620,7 @@
     </row>
     <row r="152" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B152">
         <v>2.2000000000000002</v>
@@ -40886,7 +40886,7 @@
     </row>
     <row r="153" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B153">
         <v>2</v>
@@ -41152,7 +41152,7 @@
     </row>
     <row r="154" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B154">
         <v>2.6</v>
@@ -41418,7 +41418,7 @@
     </row>
     <row r="155" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B155">
         <v>3.25</v>
@@ -41684,7 +41684,7 @@
     </row>
     <row r="156" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B156">
         <v>2.8</v>
@@ -41950,7 +41950,7 @@
     </row>
     <row r="157" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B157">
         <v>2</v>
@@ -42216,7 +42216,7 @@
     </row>
     <row r="158" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B158">
         <v>2.25</v>
@@ -42482,7 +42482,7 @@
     </row>
     <row r="159" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B159">
         <v>1.5</v>
@@ -42748,7 +42748,7 @@
     </row>
     <row r="160" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B160">
         <v>2</v>
@@ -43014,7 +43014,7 @@
     </row>
     <row r="161" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B161">
         <v>1.5</v>
@@ -43280,7 +43280,7 @@
     </row>
     <row r="162" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B162">
         <v>1.75</v>
@@ -43546,7 +43546,7 @@
     </row>
     <row r="163" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B163">
         <v>3</v>
@@ -43812,7 +43812,7 @@
     </row>
     <row r="164" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B164">
         <v>2.2000000000000002</v>
@@ -44078,7 +44078,7 @@
     </row>
     <row r="165" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B165">
         <v>2.666666666666667</v>
@@ -44344,7 +44344,7 @@
     </row>
     <row r="166" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B166">
         <v>1.75</v>
@@ -44610,7 +44610,7 @@
     </row>
     <row r="167" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B167">
         <v>3.75</v>
@@ -44876,7 +44876,7 @@
     </row>
     <row r="168" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B168">
         <v>1.25</v>
@@ -45142,7 +45142,7 @@
     </row>
     <row r="169" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B169">
         <v>3</v>
@@ -45408,7 +45408,7 @@
     </row>
     <row r="170" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B170">
         <v>3</v>
@@ -45674,7 +45674,7 @@
     </row>
     <row r="171" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B171">
         <v>1.75</v>
@@ -45940,7 +45940,7 @@
     </row>
     <row r="172" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B172">
         <v>3.25</v>
@@ -46206,7 +46206,7 @@
     </row>
     <row r="173" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B173">
         <v>2.5</v>
@@ -46472,7 +46472,7 @@
     </row>
     <row r="174" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B174">
         <v>3.25</v>
@@ -46738,7 +46738,7 @@
     </row>
     <row r="175" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B175">
         <v>3.4</v>
@@ -47004,7 +47004,7 @@
     </row>
     <row r="176" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B176">
         <v>2.25</v>
@@ -47270,7 +47270,7 @@
     </row>
     <row r="177" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B177">
         <v>4</v>
@@ -47536,7 +47536,7 @@
     </row>
     <row r="178" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B178">
         <v>2.5</v>
@@ -47802,7 +47802,7 @@
     </row>
     <row r="179" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B179">
         <v>2.25</v>
@@ -48068,7 +48068,7 @@
     </row>
     <row r="180" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B180">
         <v>2.25</v>
@@ -48334,7 +48334,7 @@
     </row>
     <row r="181" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B181">
         <v>3.666666666666667</v>
@@ -48600,7 +48600,7 @@
     </row>
     <row r="182" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B182">
         <v>2.25</v>
@@ -48866,7 +48866,7 @@
     </row>
     <row r="183" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B183">
         <v>4.333333333333333</v>
@@ -49132,7 +49132,7 @@
     </row>
     <row r="184" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B184">
         <v>2</v>
@@ -49398,7 +49398,7 @@
     </row>
     <row r="185" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B185">
         <v>2.75</v>
@@ -49664,7 +49664,7 @@
     </row>
     <row r="186" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B186">
         <v>2.5</v>
@@ -49930,7 +49930,7 @@
     </row>
     <row r="187" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B187">
         <v>2.5</v>
@@ -50196,7 +50196,7 @@
     </row>
     <row r="188" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B188">
         <v>1.666666666666667</v>
@@ -50462,7 +50462,7 @@
     </row>
     <row r="189" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B189">
         <v>2.5</v>
@@ -50728,7 +50728,7 @@
     </row>
     <row r="190" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B190">
         <v>3.25</v>
@@ -50994,7 +50994,7 @@
     </row>
     <row r="191" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B191">
         <v>2</v>
@@ -51260,7 +51260,7 @@
     </row>
     <row r="192" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B192">
         <v>4.25</v>
@@ -51526,7 +51526,7 @@
     </row>
     <row r="193" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B193">
         <v>2.8</v>
@@ -51792,7 +51792,7 @@
     </row>
     <row r="194" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B194">
         <v>2.4</v>
@@ -52058,7 +52058,7 @@
     </row>
     <row r="195" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B195">
         <v>4</v>
@@ -52324,7 +52324,7 @@
     </row>
     <row r="196" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B196">
         <v>3.333333333333333</v>
@@ -52590,7 +52590,7 @@
     </row>
     <row r="197" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B197">
         <v>2.6</v>
@@ -52856,7 +52856,7 @@
     </row>
     <row r="198" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B198">
         <v>2.8</v>
@@ -53122,7 +53122,7 @@
     </row>
     <row r="199" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B199">
         <v>2</v>
@@ -53388,7 +53388,7 @@
     </row>
     <row r="200" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B200">
         <v>2.25</v>
@@ -53654,7 +53654,7 @@
     </row>
     <row r="201" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B201">
         <v>3</v>
@@ -53920,7 +53920,7 @@
     </row>
     <row r="202" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B202">
         <v>2.25</v>
@@ -54186,26 +54186,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="AU1:AW1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="BD1:BF1"/>
-    <mergeCell ref="BG1:BI1"/>
     <mergeCell ref="BY1:CA1"/>
     <mergeCell ref="CB1:CD1"/>
     <mergeCell ref="CE1:CG1"/>
@@ -54215,6 +54195,26 @@
     <mergeCell ref="BP1:BR1"/>
     <mergeCell ref="BS1:BU1"/>
     <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>